<commit_message>
Created a new Training set, corrected a mistake in the data aggregation process
</commit_message>
<xml_diff>
--- a/TrainingSet.xlsx
+++ b/TrainingSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Erik\Downloads\b;\DS\SmiteSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E0F220-BD0B-45AB-A0C0-84FF62774C5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E0FCED-B59B-4D35-9CB6-7D4B1810A046}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA6FE912-4576-4140-B69C-9BECECFBBE00}"/>
+    <workbookView xWindow="7245" yWindow="2220" windowWidth="20040" windowHeight="10035" xr2:uid="{FA6FE912-4576-4140-B69C-9BECECFBBE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FDA0AE-64AE-49AA-AB31-3659D432EFDE}">
   <dimension ref="A1:J385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>